<commit_message>
14-03-2023 -> Scripting DPLKKPS149-001, DPLKKPS150-001, DPLKKPS150-002, 15-03-2023 -> Scripting DPLKKEU028-001 16-03-2023 -> Scripting DPLKKEU026-001 17-03-2023 -> Scripting DPLKKEU028-001 Fix
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKEU026-001 - Keuangan - Transaksi - Entry Teller Kolektif.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKEU026-001 - Keuangan - Transaksi - Entry Teller Kolektif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45286AB1-D4A1-4A98-B71C-72F019E0B9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A8AE20-94F1-454F-93EC-435474073172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>RUN</t>
   </si>
@@ -100,36 +100,48 @@
     <t>TUJUAN_TRANSAKSI</t>
   </si>
   <si>
-    <t>UP032303000009</t>
-  </si>
-  <si>
     <t>KEU.KEP.TRX.068/11 diterima</t>
   </si>
   <si>
-    <t>Username : 31674;
+    <t>Data Penerimaan Teller Kolektif berhasil dibuat</t>
+  </si>
+  <si>
+    <t>Kas Perusahaan</t>
+  </si>
+  <si>
+    <t>Pemindahan Dana</t>
+  </si>
+  <si>
+    <t>PASSWORD_ICONS</t>
+  </si>
+  <si>
+    <t>KODE_CABANG_ICONS</t>
+  </si>
+  <si>
+    <t>NOMOR_TERMINAL_ICONS</t>
+  </si>
+  <si>
+    <t>259</t>
+  </si>
+  <si>
+    <t>UP032303000030</t>
+  </si>
+  <si>
+    <t>Username : 12773;
 Password : bni1234;
 Role : 39 - Teller;
-Upload ID : UP032303000009;
-Nominal Penerimaan : 273019274100;
+Upload ID : UP032303000030;
+Nominal Penerimaan : 121.000.000,00;
 Keterangan : KEU.KEP.TRX.068/11 diterima;
-Sumber Dana : ;
-Tujuan Transaksi :;</t>
-  </si>
-  <si>
-    <t>Data Penerimaan Teller Kolektif berhasil dibuat</t>
-  </si>
-  <si>
-    <t>Kas Perusahaan</t>
-  </si>
-  <si>
-    <t>Pemindahan Dana</t>
+Sumber Dana : Kas Perusahaan;
+Tujuan Transaksi : Pemindahan Dana;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +182,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,18 +214,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -211,9 +235,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -232,8 +253,16 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653A54F0-D01B-49C0-BB41-F0FC7D2164BA}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,9 +593,9 @@
     <col min="16" max="16" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -574,123 +603,138 @@
     <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="S1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:24" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4">
+        <v>12773</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="9">
+        <v>121000000</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="5">
-        <v>31674</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="11">
-        <v>2730192741</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="9"/>
+      <c r="S2" s="13">
+        <v>1</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="13">
+        <v>259</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>